<commit_message>
Mini Assignment Week 3 Mock Up Preliminary Data Analysis
This Excel document contains two sheets containing mock up data. The first sheet is a shortened version of what I want my (wide to) long data to look like, with some of the categories of analysis/descriptive statistics that I eventually want to code with R. And the second sheet contains simple drawings of key plots I would like to include in my report. These plots would describe 1) by issue, which issues passed and which issues were rejected relative to the 2/3 quorum rule in the Constitutional Convention; 2 and 3) by delegate (in the REG and SUBS phases), how many issues they passed. @nrdowling @hjennybo
</commit_message>
<xml_diff>
--- a/Mock Up Preliminary Analysis .xlsx
+++ b/Mock Up Preliminary Analysis .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaalvarez/Documents/GitHub/ChileanCCRollCallVotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D00FBD-AEF0-1D4A-BA01-2AF6AE323C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEDC00A-9DCA-8A41-B7F2-33FA064068A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="460" windowWidth="24140" windowHeight="16320" activeTab="1" xr2:uid="{CBFA4F2C-1E91-3D4F-BE56-8D68F9953033}"/>
+    <workbookView xWindow="3020" yWindow="460" windowWidth="24140" windowHeight="16320" xr2:uid="{CBFA4F2C-1E91-3D4F-BE56-8D68F9953033}"/>
   </bookViews>
   <sheets>
     <sheet name="Mock Up Data for Stats" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +269,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -375,18 +381,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,8 +618,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>190496</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="3" name="Ink 2">
@@ -634,7 +638,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="3" name="Ink 2">
@@ -679,8 +683,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>40820</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="6" name="Ink 5">
@@ -699,7 +703,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="6" name="Ink 5">
@@ -744,8 +748,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>129296</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="9" name="Ink 8">
@@ -764,7 +768,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="9" name="Ink 8">
@@ -809,8 +813,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>160531</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="10" name="Ink 9">
@@ -829,7 +833,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="10" name="Ink 9">
@@ -874,8 +878,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>165888</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="61" name="Ink 60">
@@ -894,7 +898,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="61" name="Ink 60">
@@ -939,8 +943,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>26770</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="74" name="Ink 73">
@@ -959,7 +963,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="74" name="Ink 73">
@@ -1004,8 +1008,8 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>182088</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="75" name="Ink 74">
@@ -1024,7 +1028,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="75" name="Ink 74">
@@ -1069,8 +1073,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>149764</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="76" name="Ink 75">
@@ -1089,7 +1093,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="76" name="Ink 75">
@@ -1134,8 +1138,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>150907</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="85" name="Ink 84">
@@ -1154,7 +1158,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="85" name="Ink 84">
@@ -1194,8 +1198,8 @@
       <xdr:rowOff>110618</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3741480" cy="416520"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="86" name="Ink 85">
@@ -1214,7 +1218,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="86" name="Ink 85">
@@ -1254,8 +1258,8 @@
       <xdr:rowOff>52930</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="123120" cy="360"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="87" name="Ink 86">
@@ -1274,7 +1278,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="87" name="Ink 86">
@@ -1314,8 +1318,8 @@
       <xdr:rowOff>81668</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="573480" cy="224280"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="88" name="Ink 87">
@@ -1334,7 +1338,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="88" name="Ink 87">
@@ -1374,8 +1378,8 @@
       <xdr:rowOff>122625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="253800" cy="267480"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="89" name="Ink 88">
@@ -1394,7 +1398,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="89" name="Ink 88">
@@ -1434,8 +1438,8 @@
       <xdr:rowOff>187256</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3741480" cy="416520"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="91" name="Ink 90">
@@ -1454,7 +1458,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="91" name="Ink 90">
@@ -1494,8 +1498,8 @@
       <xdr:rowOff>206206</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="123120" cy="360"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="92" name="Ink 91">
@@ -1514,7 +1518,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="92" name="Ink 91">
@@ -1554,8 +1558,8 @@
       <xdr:rowOff>169254</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="573480" cy="224280"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="93" name="Ink 92">
@@ -1574,7 +1578,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="93" name="Ink 92">
@@ -2819,8 +2823,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>183616</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId35">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="127" name="Ink 126">
@@ -2839,7 +2843,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="127" name="Ink 126">
@@ -2884,8 +2888,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>96170</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId37">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="129" name="Ink 128">
@@ -2904,7 +2908,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="129" name="Ink 128">
@@ -2949,8 +2953,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>152828</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId39">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="137" name="Ink 136">
@@ -2969,7 +2973,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="137" name="Ink 136">
@@ -3014,8 +3018,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>20365</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId41">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="142" name="Ink 141">
@@ -3034,7 +3038,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="142" name="Ink 141">
@@ -3079,8 +3083,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>126050</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId43">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="143" name="Ink 142">
@@ -3099,7 +3103,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="143" name="Ink 142">
@@ -3144,8 +3148,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>158090</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId45">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="146" name="Ink 145">
@@ -3164,7 +3168,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="146" name="Ink 145">
@@ -3209,8 +3213,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>173570</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId47">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="147" name="Ink 146">
@@ -3229,7 +3233,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="147" name="Ink 146">
@@ -3274,8 +3278,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>179690</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId49">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="148" name="Ink 147">
@@ -3294,7 +3298,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="148" name="Ink 147">
@@ -3339,8 +3343,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>193730</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId51">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="151" name="Ink 150">
@@ -3359,7 +3363,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="151" name="Ink 150">
@@ -3404,8 +3408,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>42592</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId53">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="166" name="Ink 165">
@@ -3424,7 +3428,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="166" name="Ink 165">
@@ -3469,8 +3473,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>189770</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId55">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="169" name="Ink 168">
@@ -3489,7 +3493,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="169" name="Ink 168">
@@ -3534,8 +3538,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>165650</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId57">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="170" name="Ink 169">
@@ -3554,7 +3558,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="170" name="Ink 169">
@@ -3599,8 +3603,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>165650</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId59">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="171" name="Ink 170">
@@ -3619,7 +3623,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="171" name="Ink 170">
@@ -3664,8 +3668,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>157010</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId60">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="172" name="Ink 171">
@@ -3684,7 +3688,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="172" name="Ink 171">
@@ -3729,8 +3733,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>54112</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId61">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="179" name="Ink 178">
@@ -3749,7 +3753,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="179" name="Ink 178">
@@ -5785,8 +5789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6052B15-2C46-DA42-B75F-917C062A0779}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7052,6 +7056,20 @@
         <v>43</v>
       </c>
     </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+    </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>46</v>
@@ -7066,8 +7084,8 @@
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="15" t="s">
+      <c r="L36" s="13"/>
+      <c r="M36" s="14" t="s">
         <v>45</v>
       </c>
     </row>
@@ -7085,8 +7103,6 @@
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
       <c r="K37" s="12"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7098,7 +7114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582384FC-8BB4-3B4D-9657-021FE1E9A445}">
   <dimension ref="A2:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+    <sheetView zoomScale="116" workbookViewId="0">
       <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
@@ -7110,66 +7126,60 @@
     <col min="11" max="11" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J7" s="18" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K20" s="13"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="I21" s="16"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="I21" s="19"/>
-      <c r="K21" s="13"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="I22" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="K22" s="13"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="H28" s="21" t="s">
+      <c r="H28" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C42" s="22" t="s">
+      <c r="C42" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="K42" s="22" t="s">
+      <c r="K42" s="19" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>